<commit_message>
add small and big matrix
</commit_message>
<xml_diff>
--- a/experiment.xlsx
+++ b/experiment.xlsx
@@ -187,7 +187,7 @@
   <dimension ref="A1:S133"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M124" activeCellId="0" sqref="M124"/>
+      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -268,7 +268,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -300,31 +300,31 @@
         <v>22</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
@@ -356,31 +356,31 @@
         <v>22</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1</v>
       </c>
@@ -412,31 +412,31 @@
         <v>22</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
@@ -468,31 +468,31 @@
         <v>22</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N6" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1</v>
       </c>
@@ -524,31 +524,31 @@
         <v>22</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>1</v>
       </c>
@@ -580,31 +580,31 @@
         <v>22</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>1</v>
       </c>
@@ -636,31 +636,31 @@
         <v>22</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N9" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O9" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P9" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q9" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1</v>
       </c>
@@ -692,25 +692,25 @@
         <v>22</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S10" s="0" t="n">
         <v>0</v>
@@ -762,25 +762,25 @@
         <v>22</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S12" s="0" t="n">
         <v>0</v>
@@ -818,25 +818,25 @@
         <v>22</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S13" s="0" t="n">
         <v>0</v>
@@ -874,25 +874,25 @@
         <v>22</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S14" s="0" t="n">
         <v>0</v>
@@ -930,25 +930,25 @@
         <v>22</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S15" s="0" t="n">
         <v>0</v>
@@ -986,25 +986,25 @@
         <v>22</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N16" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P16" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q16" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S16" s="0" t="n">
         <v>0</v>
@@ -1042,25 +1042,25 @@
         <v>22</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N17" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O17" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P17" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q17" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S17" s="0" t="n">
         <v>0</v>
@@ -1098,25 +1098,25 @@
         <v>22</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N18" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P18" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q18" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S18" s="0" t="n">
         <v>0</v>
@@ -1154,25 +1154,25 @@
         <v>22</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M19" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N19" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P19" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q19" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S19" s="0" t="n">
         <v>0</v>
@@ -1210,25 +1210,25 @@
         <v>22</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N20" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O20" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q20" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S20" s="0" t="n">
         <v>0</v>
@@ -1266,25 +1266,25 @@
         <v>22</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M21" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N21" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O21" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P21" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q21" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S21" s="0" t="n">
         <v>0</v>
@@ -1322,25 +1322,25 @@
         <v>22</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M22" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N22" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P22" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q22" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S22" s="0" t="n">
         <v>0</v>
@@ -1378,25 +1378,25 @@
         <v>22</v>
       </c>
       <c r="K23" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M23" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N23" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O23" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P23" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q23" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S23" s="0" t="n">
         <v>0</v>
@@ -1434,25 +1434,25 @@
         <v>22</v>
       </c>
       <c r="K24" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N24" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O24" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P24" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q24" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S24" s="0" t="n">
         <v>0</v>
@@ -1490,25 +1490,25 @@
         <v>22</v>
       </c>
       <c r="K25" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N25" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O25" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P25" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q25" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S25" s="0" t="n">
         <v>0</v>
@@ -1546,25 +1546,25 @@
         <v>22</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M26" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O26" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P26" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q26" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S26" s="0" t="n">
         <v>0</v>
@@ -1602,25 +1602,25 @@
         <v>22</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M27" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N27" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O27" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P27" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q27" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S27" s="0" t="n">
         <v>0</v>
@@ -1658,25 +1658,25 @@
         <v>22</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M28" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N28" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O28" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P28" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q28" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S28" s="0" t="n">
         <v>0</v>
@@ -1714,25 +1714,25 @@
         <v>22</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M29" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N29" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O29" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P29" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q29" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S29" s="0" t="n">
         <v>0</v>
@@ -1770,25 +1770,25 @@
         <v>22</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M30" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N30" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O30" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P30" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q30" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S30" s="0" t="n">
         <v>0</v>
@@ -1826,25 +1826,25 @@
         <v>22</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M31" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N31" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O31" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P31" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q31" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S31" s="0" t="n">
         <v>0</v>
@@ -1882,25 +1882,25 @@
         <v>22</v>
       </c>
       <c r="K32" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M32" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N32" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O32" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P32" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q32" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S32" s="0" t="n">
         <v>0</v>
@@ -1938,25 +1938,25 @@
         <v>22</v>
       </c>
       <c r="K33" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L33" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M33" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N33" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O33" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P33" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q33" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S33" s="0" t="n">
         <v>0</v>
@@ -1994,25 +1994,25 @@
         <v>22</v>
       </c>
       <c r="K34" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L34" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M34" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N34" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O34" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P34" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q34" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S34" s="0" t="n">
         <v>0</v>
@@ -2050,25 +2050,25 @@
         <v>22</v>
       </c>
       <c r="K35" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L35" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M35" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N35" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O35" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P35" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q35" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S35" s="0" t="n">
         <v>0</v>
@@ -2106,25 +2106,25 @@
         <v>22</v>
       </c>
       <c r="K36" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L36" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M36" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N36" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O36" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P36" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q36" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S36" s="0" t="n">
         <v>0</v>
@@ -2162,25 +2162,25 @@
         <v>22</v>
       </c>
       <c r="K37" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L37" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M37" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N37" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O37" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P37" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q37" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S37" s="0" t="n">
         <v>0</v>
@@ -2218,25 +2218,25 @@
         <v>22</v>
       </c>
       <c r="K38" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L38" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M38" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N38" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O38" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P38" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q38" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S38" s="0" t="n">
         <v>0</v>
@@ -2274,25 +2274,25 @@
         <v>22</v>
       </c>
       <c r="K39" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L39" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M39" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N39" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O39" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P39" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q39" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S39" s="0" t="n">
         <v>0</v>
@@ -2330,25 +2330,25 @@
         <v>22</v>
       </c>
       <c r="K40" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L40" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M40" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N40" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O40" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P40" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q40" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S40" s="0" t="n">
         <v>0</v>
@@ -2386,25 +2386,25 @@
         <v>22</v>
       </c>
       <c r="K41" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L41" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M41" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N41" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O41" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P41" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q41" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S41" s="0" t="n">
         <v>0</v>
@@ -2442,25 +2442,25 @@
         <v>22</v>
       </c>
       <c r="K42" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L42" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M42" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N42" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O42" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P42" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q42" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S42" s="0" t="n">
         <v>0</v>
@@ -2498,25 +2498,25 @@
         <v>22</v>
       </c>
       <c r="K43" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L43" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M43" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N43" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O43" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P43" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q43" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S43" s="0" t="n">
         <v>0</v>
@@ -2554,25 +2554,25 @@
         <v>22</v>
       </c>
       <c r="K44" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M44" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N44" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O44" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P44" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q44" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S44" s="0" t="n">
         <v>0</v>
@@ -2610,25 +2610,25 @@
         <v>22</v>
       </c>
       <c r="K45" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L45" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M45" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N45" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O45" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P45" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q45" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S45" s="0" t="n">
         <v>0</v>
@@ -2666,25 +2666,25 @@
         <v>22</v>
       </c>
       <c r="K46" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L46" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M46" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N46" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O46" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P46" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q46" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S46" s="0" t="n">
         <v>0</v>
@@ -2722,25 +2722,25 @@
         <v>22</v>
       </c>
       <c r="K47" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L47" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M47" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N47" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O47" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P47" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q47" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S47" s="0" t="n">
         <v>0</v>
@@ -2778,25 +2778,25 @@
         <v>22</v>
       </c>
       <c r="K48" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L48" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M48" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N48" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O48" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P48" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q48" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S48" s="0" t="n">
         <v>0</v>
@@ -2834,25 +2834,25 @@
         <v>22</v>
       </c>
       <c r="K49" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L49" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M49" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N49" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O49" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P49" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q49" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S49" s="0" t="n">
         <v>0</v>
@@ -2890,25 +2890,25 @@
         <v>22</v>
       </c>
       <c r="K50" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L50" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M50" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N50" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O50" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P50" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q50" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S50" s="0" t="n">
         <v>0</v>
@@ -2946,25 +2946,25 @@
         <v>22</v>
       </c>
       <c r="K51" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L51" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M51" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N51" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O51" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P51" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q51" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S51" s="0" t="n">
         <v>0</v>
@@ -3016,25 +3016,25 @@
         <v>22</v>
       </c>
       <c r="K53" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L53" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M53" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N53" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O53" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P53" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q53" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S53" s="0" t="n">
         <v>0</v>
@@ -3072,25 +3072,25 @@
         <v>22</v>
       </c>
       <c r="K54" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L54" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M54" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N54" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O54" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P54" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q54" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S54" s="0" t="n">
         <v>0</v>
@@ -3128,25 +3128,25 @@
         <v>22</v>
       </c>
       <c r="K55" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L55" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M55" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N55" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O55" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P55" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q55" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S55" s="0" t="n">
         <v>0</v>
@@ -3184,25 +3184,25 @@
         <v>22</v>
       </c>
       <c r="K56" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L56" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M56" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N56" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O56" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P56" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q56" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S56" s="0" t="n">
         <v>0</v>
@@ -3240,25 +3240,25 @@
         <v>22</v>
       </c>
       <c r="K57" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L57" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M57" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N57" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O57" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P57" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q57" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S57" s="0" t="n">
         <v>0</v>
@@ -3296,25 +3296,25 @@
         <v>22</v>
       </c>
       <c r="K58" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L58" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M58" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N58" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O58" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P58" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q58" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S58" s="0" t="n">
         <v>0</v>
@@ -3352,25 +3352,25 @@
         <v>22</v>
       </c>
       <c r="K59" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L59" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M59" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N59" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O59" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P59" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q59" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S59" s="0" t="n">
         <v>0</v>
@@ -3408,25 +3408,25 @@
         <v>22</v>
       </c>
       <c r="K60" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L60" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M60" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N60" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O60" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P60" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q60" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S60" s="0" t="n">
         <v>0</v>
@@ -3464,25 +3464,25 @@
         <v>22</v>
       </c>
       <c r="K61" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L61" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M61" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N61" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O61" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P61" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q61" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S61" s="0" t="n">
         <v>0</v>
@@ -3520,25 +3520,25 @@
         <v>22</v>
       </c>
       <c r="K62" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L62" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M62" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N62" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O62" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P62" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q62" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S62" s="0" t="n">
         <v>0</v>
@@ -3576,25 +3576,25 @@
         <v>22</v>
       </c>
       <c r="K63" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L63" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M63" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N63" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O63" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P63" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q63" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S63" s="0" t="n">
         <v>0</v>
@@ -3632,25 +3632,25 @@
         <v>22</v>
       </c>
       <c r="K64" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L64" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M64" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N64" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O64" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P64" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q64" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S64" s="0" t="n">
         <v>0</v>
@@ -3688,25 +3688,25 @@
         <v>22</v>
       </c>
       <c r="K65" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L65" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M65" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N65" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O65" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P65" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q65" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S65" s="0" t="n">
         <v>0</v>
@@ -3744,25 +3744,25 @@
         <v>22</v>
       </c>
       <c r="K66" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L66" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M66" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N66" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O66" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P66" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q66" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S66" s="0" t="n">
         <v>0</v>
@@ -3800,25 +3800,25 @@
         <v>22</v>
       </c>
       <c r="K67" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L67" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M67" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N67" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O67" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P67" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q67" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S67" s="0" t="n">
         <v>0</v>
@@ -3856,25 +3856,25 @@
         <v>22</v>
       </c>
       <c r="K68" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L68" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M68" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N68" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O68" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P68" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q68" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S68" s="0" t="n">
         <v>0</v>
@@ -3912,25 +3912,25 @@
         <v>22</v>
       </c>
       <c r="K69" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L69" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M69" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N69" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O69" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P69" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q69" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S69" s="0" t="n">
         <v>0</v>
@@ -3968,25 +3968,25 @@
         <v>22</v>
       </c>
       <c r="K70" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L70" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M70" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N70" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O70" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P70" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q70" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S70" s="0" t="n">
         <v>0</v>
@@ -4024,25 +4024,25 @@
         <v>22</v>
       </c>
       <c r="K71" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L71" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M71" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N71" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O71" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P71" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q71" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S71" s="0" t="n">
         <v>0</v>
@@ -4080,25 +4080,25 @@
         <v>22</v>
       </c>
       <c r="K72" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L72" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M72" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N72" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O72" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P72" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q72" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S72" s="0" t="n">
         <v>0</v>
@@ -4136,25 +4136,25 @@
         <v>22</v>
       </c>
       <c r="K73" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L73" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M73" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N73" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O73" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P73" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q73" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S73" s="0" t="n">
         <v>0</v>
@@ -4192,25 +4192,25 @@
         <v>22</v>
       </c>
       <c r="K74" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L74" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M74" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N74" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O74" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P74" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q74" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S74" s="0" t="n">
         <v>0</v>
@@ -4248,25 +4248,25 @@
         <v>22</v>
       </c>
       <c r="K75" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L75" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M75" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N75" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O75" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P75" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q75" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S75" s="0" t="n">
         <v>0</v>
@@ -4304,25 +4304,25 @@
         <v>22</v>
       </c>
       <c r="K76" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L76" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M76" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N76" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O76" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P76" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q76" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S76" s="0" t="n">
         <v>0</v>
@@ -4360,25 +4360,25 @@
         <v>22</v>
       </c>
       <c r="K77" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L77" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M77" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N77" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O77" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P77" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q77" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S77" s="0" t="n">
         <v>0</v>
@@ -4416,25 +4416,25 @@
         <v>22</v>
       </c>
       <c r="K78" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L78" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M78" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N78" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O78" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P78" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q78" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S78" s="0" t="n">
         <v>0</v>
@@ -4472,25 +4472,25 @@
         <v>22</v>
       </c>
       <c r="K79" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L79" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M79" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N79" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O79" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P79" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q79" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S79" s="0" t="n">
         <v>0</v>
@@ -4528,25 +4528,25 @@
         <v>22</v>
       </c>
       <c r="K80" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L80" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M80" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N80" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O80" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P80" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q80" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S80" s="0" t="n">
         <v>0</v>
@@ -4584,25 +4584,25 @@
         <v>22</v>
       </c>
       <c r="K81" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L81" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M81" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N81" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O81" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P81" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q81" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S81" s="0" t="n">
         <v>0</v>
@@ -4640,25 +4640,25 @@
         <v>22</v>
       </c>
       <c r="K82" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L82" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M82" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N82" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O82" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P82" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q82" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S82" s="0" t="n">
         <v>0</v>
@@ -4696,25 +4696,25 @@
         <v>22</v>
       </c>
       <c r="K83" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L83" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M83" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N83" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O83" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P83" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q83" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S83" s="0" t="n">
         <v>0</v>
@@ -4752,25 +4752,25 @@
         <v>22</v>
       </c>
       <c r="K84" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L84" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M84" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N84" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O84" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P84" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q84" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S84" s="0" t="n">
         <v>0</v>
@@ -4808,25 +4808,25 @@
         <v>22</v>
       </c>
       <c r="K85" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L85" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M85" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N85" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O85" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P85" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q85" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S85" s="0" t="n">
         <v>0</v>
@@ -4864,25 +4864,25 @@
         <v>22</v>
       </c>
       <c r="K86" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L86" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M86" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N86" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O86" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P86" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q86" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S86" s="0" t="n">
         <v>0</v>
@@ -4920,25 +4920,25 @@
         <v>22</v>
       </c>
       <c r="K87" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L87" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M87" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N87" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O87" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P87" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q87" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S87" s="0" t="n">
         <v>0</v>
@@ -4976,25 +4976,25 @@
         <v>22</v>
       </c>
       <c r="K88" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L88" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M88" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N88" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O88" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P88" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q88" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S88" s="0" t="n">
         <v>0</v>
@@ -5032,25 +5032,25 @@
         <v>22</v>
       </c>
       <c r="K89" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L89" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M89" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N89" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O89" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P89" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q89" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S89" s="0" t="n">
         <v>0</v>
@@ -5088,25 +5088,25 @@
         <v>22</v>
       </c>
       <c r="K90" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L90" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M90" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N90" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O90" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P90" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q90" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S90" s="0" t="n">
         <v>0</v>
@@ -5144,25 +5144,25 @@
         <v>22</v>
       </c>
       <c r="K91" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L91" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M91" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N91" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O91" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P91" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q91" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S91" s="0" t="n">
         <v>0</v>
@@ -5200,25 +5200,25 @@
         <v>22</v>
       </c>
       <c r="K92" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L92" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M92" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N92" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O92" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P92" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q92" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S92" s="0" t="n">
         <v>0</v>
@@ -5270,25 +5270,25 @@
         <v>22</v>
       </c>
       <c r="K94" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L94" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M94" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N94" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O94" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P94" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q94" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S94" s="0" t="n">
         <v>0</v>
@@ -5326,25 +5326,25 @@
         <v>22</v>
       </c>
       <c r="K95" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L95" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M95" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N95" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O95" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P95" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q95" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S95" s="0" t="n">
         <v>0</v>
@@ -5382,25 +5382,25 @@
         <v>22</v>
       </c>
       <c r="K96" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L96" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M96" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N96" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O96" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P96" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q96" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S96" s="0" t="n">
         <v>0</v>
@@ -5438,25 +5438,25 @@
         <v>22</v>
       </c>
       <c r="K97" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L97" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M97" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N97" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O97" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P97" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q97" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S97" s="0" t="n">
         <v>0</v>
@@ -5494,25 +5494,25 @@
         <v>22</v>
       </c>
       <c r="K98" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L98" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M98" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N98" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O98" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P98" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q98" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S98" s="0" t="n">
         <v>0</v>
@@ -5550,25 +5550,25 @@
         <v>22</v>
       </c>
       <c r="K99" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L99" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M99" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N99" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O99" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P99" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q99" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S99" s="0" t="n">
         <v>0</v>
@@ -5606,25 +5606,25 @@
         <v>22</v>
       </c>
       <c r="K100" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L100" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M100" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N100" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O100" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P100" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q100" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S100" s="0" t="n">
         <v>0</v>
@@ -5662,25 +5662,25 @@
         <v>22</v>
       </c>
       <c r="K101" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L101" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M101" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N101" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O101" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P101" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q101" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S101" s="0" t="n">
         <v>0</v>
@@ -5718,25 +5718,25 @@
         <v>22</v>
       </c>
       <c r="K102" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L102" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M102" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N102" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O102" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P102" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q102" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S102" s="0" t="n">
         <v>0</v>
@@ -5774,25 +5774,25 @@
         <v>22</v>
       </c>
       <c r="K103" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L103" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M103" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N103" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O103" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P103" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q103" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S103" s="0" t="n">
         <v>0</v>
@@ -5830,25 +5830,25 @@
         <v>22</v>
       </c>
       <c r="K104" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L104" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M104" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N104" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O104" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P104" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q104" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S104" s="0" t="n">
         <v>0</v>
@@ -5886,25 +5886,25 @@
         <v>22</v>
       </c>
       <c r="K105" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L105" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M105" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N105" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O105" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P105" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q105" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>0</v>
@@ -5942,25 +5942,25 @@
         <v>22</v>
       </c>
       <c r="K106" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L106" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M106" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N106" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O106" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P106" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q106" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>0</v>
@@ -5998,25 +5998,25 @@
         <v>22</v>
       </c>
       <c r="K107" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L107" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M107" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N107" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O107" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P107" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q107" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>0</v>
@@ -6054,25 +6054,25 @@
         <v>22</v>
       </c>
       <c r="K108" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L108" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M108" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N108" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O108" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P108" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q108" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S108" s="0" t="n">
         <v>0</v>
@@ -6110,25 +6110,25 @@
         <v>22</v>
       </c>
       <c r="K109" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L109" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M109" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N109" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O109" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P109" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q109" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S109" s="0" t="n">
         <v>0</v>
@@ -6166,25 +6166,25 @@
         <v>22</v>
       </c>
       <c r="K110" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L110" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M110" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N110" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O110" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P110" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q110" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S110" s="0" t="n">
         <v>0</v>
@@ -6222,25 +6222,25 @@
         <v>22</v>
       </c>
       <c r="K111" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L111" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M111" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N111" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O111" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P111" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q111" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S111" s="0" t="n">
         <v>0</v>
@@ -6278,25 +6278,25 @@
         <v>22</v>
       </c>
       <c r="K112" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L112" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M112" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N112" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O112" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P112" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q112" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S112" s="0" t="n">
         <v>0</v>
@@ -6334,25 +6334,25 @@
         <v>22</v>
       </c>
       <c r="K113" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L113" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M113" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N113" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O113" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P113" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q113" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S113" s="0" t="n">
         <v>0</v>
@@ -6390,25 +6390,25 @@
         <v>22</v>
       </c>
       <c r="K114" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L114" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M114" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N114" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O114" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P114" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q114" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S114" s="0" t="n">
         <v>0</v>
@@ -6446,25 +6446,25 @@
         <v>22</v>
       </c>
       <c r="K115" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L115" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M115" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N115" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O115" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P115" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q115" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S115" s="0" t="n">
         <v>0</v>
@@ -6502,25 +6502,25 @@
         <v>22</v>
       </c>
       <c r="K116" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L116" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M116" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N116" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O116" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P116" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q116" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S116" s="0" t="n">
         <v>0</v>
@@ -6558,25 +6558,25 @@
         <v>22</v>
       </c>
       <c r="K117" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L117" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M117" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N117" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O117" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P117" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q117" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S117" s="0" t="n">
         <v>0</v>
@@ -6614,25 +6614,25 @@
         <v>22</v>
       </c>
       <c r="K118" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L118" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M118" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N118" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O118" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P118" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q118" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S118" s="0" t="n">
         <v>0</v>
@@ -6670,25 +6670,25 @@
         <v>22</v>
       </c>
       <c r="K119" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L119" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M119" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N119" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O119" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P119" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q119" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S119" s="0" t="n">
         <v>0</v>
@@ -6726,25 +6726,25 @@
         <v>22</v>
       </c>
       <c r="K120" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L120" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M120" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N120" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O120" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P120" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q120" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S120" s="0" t="n">
         <v>0</v>
@@ -6782,25 +6782,25 @@
         <v>22</v>
       </c>
       <c r="K121" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L121" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M121" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N121" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O121" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P121" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q121" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S121" s="0" t="n">
         <v>0</v>
@@ -6838,25 +6838,25 @@
         <v>22</v>
       </c>
       <c r="K122" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L122" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M122" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N122" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O122" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P122" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q122" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S122" s="0" t="n">
         <v>0</v>
@@ -6894,25 +6894,25 @@
         <v>22</v>
       </c>
       <c r="K123" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L123" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M123" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N123" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O123" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P123" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q123" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S123" s="0" t="n">
         <v>0</v>
@@ -6950,25 +6950,25 @@
         <v>22</v>
       </c>
       <c r="K124" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L124" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M124" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N124" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O124" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P124" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q124" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S124" s="0" t="n">
         <v>0</v>
@@ -7006,25 +7006,25 @@
         <v>22</v>
       </c>
       <c r="K125" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L125" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M125" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N125" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O125" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P125" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q125" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S125" s="0" t="n">
         <v>0</v>
@@ -7062,25 +7062,25 @@
         <v>22</v>
       </c>
       <c r="K126" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L126" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M126" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N126" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O126" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P126" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q126" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S126" s="0" t="n">
         <v>0</v>
@@ -7118,25 +7118,25 @@
         <v>22</v>
       </c>
       <c r="K127" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L127" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M127" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N127" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O127" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P127" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q127" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S127" s="0" t="n">
         <v>0</v>
@@ -7174,25 +7174,25 @@
         <v>22</v>
       </c>
       <c r="K128" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L128" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M128" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N128" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O128" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P128" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q128" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S128" s="0" t="n">
         <v>0</v>
@@ -7230,25 +7230,25 @@
         <v>22</v>
       </c>
       <c r="K129" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L129" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M129" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N129" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O129" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P129" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q129" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S129" s="0" t="n">
         <v>0</v>
@@ -7286,25 +7286,25 @@
         <v>22</v>
       </c>
       <c r="K130" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L130" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M130" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N130" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O130" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P130" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q130" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S130" s="0" t="n">
         <v>0</v>
@@ -7342,25 +7342,25 @@
         <v>22</v>
       </c>
       <c r="K131" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L131" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M131" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N131" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O131" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P131" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q131" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S131" s="0" t="n">
         <v>0</v>
@@ -7398,25 +7398,25 @@
         <v>22</v>
       </c>
       <c r="K132" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L132" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M132" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N132" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O132" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P132" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q132" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S132" s="0" t="n">
         <v>0</v>
@@ -7454,25 +7454,25 @@
         <v>22</v>
       </c>
       <c r="K133" s="0" t="n">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="L133" s="0" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M133" s="0" t="n">
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="N133" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="O133" s="0" t="n">
-        <v>3000</v>
+        <v>3</v>
       </c>
       <c r="P133" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q133" s="0" t="n">
-        <v>1000</v>
+        <v>9</v>
       </c>
       <c r="S133" s="0" t="n">
         <v>0</v>

</xml_diff>